<commit_message>
add pre post cut column
</commit_message>
<xml_diff>
--- a/R/data_dic/data_description.xlsx
+++ b/R/data_dic/data_description.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/audhalbritter/Dropbox/Bergen/FUNDER/funcab_data/R/data_dic/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46FD55B1-5E5A-0B40-9C7F-16E00FB29E6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{059C36A1-1D94-8444-BA1A-845A005FBA7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12760" yWindow="4380" windowWidth="19620" windowHeight="17320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5260" yWindow="460" windowWidth="27620" windowHeight="21180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_description" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="147">
   <si>
     <t>TableID</t>
   </si>
@@ -520,6 +520,36 @@
   </si>
   <si>
     <t>Flag for data quality (x or DROP)</t>
+  </si>
+  <si>
+    <t>ndvi</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>pre_post_cut</t>
+  </si>
+  <si>
+    <t>Time of sampling</t>
+  </si>
+  <si>
+    <t>hh:mm</t>
+  </si>
+  <si>
+    <t>NDVI value</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Measurment was taken before or after the cut</t>
+  </si>
+  <si>
+    <t>cflux</t>
+  </si>
+  <si>
+    <t>reflectance</t>
   </si>
 </sst>
 </file>
@@ -1392,10 +1422,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E55"/>
+  <dimension ref="A1:E59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40:XFD40"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1624,7 +1654,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>48</v>
       </c>
@@ -1638,7 +1668,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>50</v>
       </c>
@@ -1652,7 +1682,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>52</v>
       </c>
@@ -1666,7 +1696,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>55</v>
       </c>
@@ -1680,7 +1710,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>57</v>
       </c>
@@ -1694,7 +1724,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>59</v>
       </c>
@@ -1708,7 +1738,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>61</v>
       </c>
@@ -1722,7 +1752,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>64</v>
       </c>
@@ -1736,7 +1766,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>66</v>
       </c>
@@ -1750,7 +1780,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>69</v>
       </c>
@@ -1764,7 +1794,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>72</v>
       </c>
@@ -1778,7 +1808,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>75</v>
       </c>
@@ -1789,7 +1819,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>77</v>
       </c>
@@ -1797,7 +1827,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>79</v>
       </c>
@@ -1811,7 +1841,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>80</v>
       </c>
@@ -1825,7 +1855,10 @@
         <v>37</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>145</v>
+      </c>
       <c r="B32" t="s">
         <v>81</v>
       </c>
@@ -2051,7 +2084,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
         <v>97</v>
       </c>
@@ -2065,7 +2098,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
         <v>98</v>
       </c>
@@ -2079,7 +2112,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
         <v>99</v>
       </c>
@@ -2093,7 +2126,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
         <v>100</v>
       </c>
@@ -2107,7 +2140,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
         <v>101</v>
       </c>
@@ -2121,7 +2154,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
         <v>102</v>
       </c>
@@ -2135,7 +2168,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
         <v>103</v>
       </c>
@@ -2147,6 +2180,59 @@
       </c>
       <c r="E55" t="s">
         <v>121</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>146</v>
+      </c>
+      <c r="B56" t="s">
+        <v>81</v>
+      </c>
+      <c r="C56" t="s">
+        <v>140</v>
+      </c>
+      <c r="D56" t="s">
+        <v>141</v>
+      </c>
+      <c r="E56" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B57" t="s">
+        <v>137</v>
+      </c>
+      <c r="C57" t="s">
+        <v>142</v>
+      </c>
+      <c r="D57" t="s">
+        <v>45</v>
+      </c>
+      <c r="E57" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B58" t="s">
+        <v>138</v>
+      </c>
+      <c r="C58" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B59" t="s">
+        <v>139</v>
+      </c>
+      <c r="C59" t="s">
+        <v>144</v>
+      </c>
+      <c r="D59" t="s">
+        <v>112</v>
+      </c>
+      <c r="E59" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix pre post cut col
</commit_message>
<xml_diff>
--- a/R/data_dic/data_description.xlsx
+++ b/R/data_dic/data_description.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/audhalbritter/Dropbox/Bergen/FUNDER/funcab_data/R/data_dic/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46FD55B1-5E5A-0B40-9C7F-16E00FB29E6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{059C36A1-1D94-8444-BA1A-845A005FBA7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12760" yWindow="4380" windowWidth="19620" windowHeight="17320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5260" yWindow="460" windowWidth="27620" windowHeight="21180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_description" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="147">
   <si>
     <t>TableID</t>
   </si>
@@ -520,6 +520,36 @@
   </si>
   <si>
     <t>Flag for data quality (x or DROP)</t>
+  </si>
+  <si>
+    <t>ndvi</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>pre_post_cut</t>
+  </si>
+  <si>
+    <t>Time of sampling</t>
+  </si>
+  <si>
+    <t>hh:mm</t>
+  </si>
+  <si>
+    <t>NDVI value</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Measurment was taken before or after the cut</t>
+  </si>
+  <si>
+    <t>cflux</t>
+  </si>
+  <si>
+    <t>reflectance</t>
   </si>
 </sst>
 </file>
@@ -1392,10 +1422,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E55"/>
+  <dimension ref="A1:E59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40:XFD40"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1624,7 +1654,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>48</v>
       </c>
@@ -1638,7 +1668,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>50</v>
       </c>
@@ -1652,7 +1682,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>52</v>
       </c>
@@ -1666,7 +1696,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>55</v>
       </c>
@@ -1680,7 +1710,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>57</v>
       </c>
@@ -1694,7 +1724,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>59</v>
       </c>
@@ -1708,7 +1738,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>61</v>
       </c>
@@ -1722,7 +1752,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>64</v>
       </c>
@@ -1736,7 +1766,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>66</v>
       </c>
@@ -1750,7 +1780,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>69</v>
       </c>
@@ -1764,7 +1794,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>72</v>
       </c>
@@ -1778,7 +1808,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>75</v>
       </c>
@@ -1789,7 +1819,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>77</v>
       </c>
@@ -1797,7 +1827,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>79</v>
       </c>
@@ -1811,7 +1841,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>80</v>
       </c>
@@ -1825,7 +1855,10 @@
         <v>37</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>145</v>
+      </c>
       <c r="B32" t="s">
         <v>81</v>
       </c>
@@ -2051,7 +2084,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
         <v>97</v>
       </c>
@@ -2065,7 +2098,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
         <v>98</v>
       </c>
@@ -2079,7 +2112,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
         <v>99</v>
       </c>
@@ -2093,7 +2126,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
         <v>100</v>
       </c>
@@ -2107,7 +2140,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
         <v>101</v>
       </c>
@@ -2121,7 +2154,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
         <v>102</v>
       </c>
@@ -2135,7 +2168,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
         <v>103</v>
       </c>
@@ -2147,6 +2180,59 @@
       </c>
       <c r="E55" t="s">
         <v>121</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>146</v>
+      </c>
+      <c r="B56" t="s">
+        <v>81</v>
+      </c>
+      <c r="C56" t="s">
+        <v>140</v>
+      </c>
+      <c r="D56" t="s">
+        <v>141</v>
+      </c>
+      <c r="E56" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B57" t="s">
+        <v>137</v>
+      </c>
+      <c r="C57" t="s">
+        <v>142</v>
+      </c>
+      <c r="D57" t="s">
+        <v>45</v>
+      </c>
+      <c r="E57" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B58" t="s">
+        <v>138</v>
+      </c>
+      <c r="C58" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B59" t="s">
+        <v>139</v>
+      </c>
+      <c r="C59" t="s">
+        <v>144</v>
+      </c>
+      <c r="D59" t="s">
+        <v>112</v>
+      </c>
+      <c r="E59" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update data description file
</commit_message>
<xml_diff>
--- a/R/data_dic/data_description.xlsx
+++ b/R/data_dic/data_description.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/audhalbritter/Dropbox/Bergen/FUNDER/funcab_data/R/data_dic/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{059C36A1-1D94-8444-BA1A-845A005FBA7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB57F51B-D25C-2A4D-97AC-51946B973AD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5260" yWindow="460" windowWidth="27620" windowHeight="21180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="39100" yWindow="460" windowWidth="27620" windowHeight="21180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_description" sheetId="1" r:id="rId1"/>
@@ -160,34 +160,19 @@
     <t>percentage</t>
   </si>
   <si>
-    <t>graminoidCov</t>
-  </si>
-  <si>
     <t>Cover of graminoids</t>
   </si>
   <si>
-    <t>forbCov</t>
-  </si>
-  <si>
     <t xml:space="preserve">Cover of forbs </t>
   </si>
   <si>
-    <t>mossCov</t>
-  </si>
-  <si>
     <t>Cover of bryophytes</t>
   </si>
   <si>
-    <t>vegetationHeight</t>
-  </si>
-  <si>
     <t>Height of vegetation</t>
   </si>
   <si>
     <t>mm</t>
-  </si>
-  <si>
-    <t>mossHeight</t>
   </si>
   <si>
     <t>Height of bryophytes</t>
@@ -550,6 +535,21 @@
   </si>
   <si>
     <t>reflectance</t>
+  </si>
+  <si>
+    <t>total_graminoids</t>
+  </si>
+  <si>
+    <t>total_forbs</t>
+  </si>
+  <si>
+    <t>total_bryophytes</t>
+  </si>
+  <si>
+    <t>vegetatio_height</t>
+  </si>
+  <si>
+    <t>moss_height</t>
   </si>
 </sst>
 </file>
@@ -1424,8 +1424,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24:C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1570,7 +1570,7 @@
         <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="D10" t="s">
         <v>31</v>
@@ -1642,10 +1642,10 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
+        <v>142</v>
+      </c>
+      <c r="C16" t="s">
         <v>46</v>
-      </c>
-      <c r="C16" t="s">
-        <v>47</v>
       </c>
       <c r="D16" t="s">
         <v>45</v>
@@ -1656,10 +1656,10 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>48</v>
+        <v>143</v>
       </c>
       <c r="C17" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D17" t="s">
         <v>45</v>
@@ -1670,10 +1670,10 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>50</v>
+        <v>144</v>
       </c>
       <c r="C18" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D18" t="s">
         <v>45</v>
@@ -1684,13 +1684,13 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>52</v>
+        <v>145</v>
       </c>
       <c r="C19" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D19" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E19" t="s">
         <v>15</v>
@@ -1698,13 +1698,13 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>55</v>
+        <v>146</v>
       </c>
       <c r="C20" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D20" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E20" t="s">
         <v>15</v>
@@ -1712,10 +1712,10 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C21" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D21" t="s">
         <v>45</v>
@@ -1726,10 +1726,10 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C22" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D22" t="s">
         <v>45</v>
@@ -1740,13 +1740,13 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D23" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E23" t="s">
         <v>8</v>
@@ -1754,10 +1754,10 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C24" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D24" t="s">
         <v>45</v>
@@ -1768,13 +1768,13 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C25" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D25" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E25" t="s">
         <v>8</v>
@@ -1782,13 +1782,13 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C26" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D26" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E26" t="s">
         <v>8</v>
@@ -1796,13 +1796,13 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C27" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D27" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E27" t="s">
         <v>15</v>
@@ -1810,10 +1810,10 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C28" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E28" t="s">
         <v>37</v>
@@ -1821,18 +1821,18 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C29" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C30" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D30" t="s">
         <v>7</v>
@@ -1843,10 +1843,10 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C31" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D31" t="s">
         <v>7</v>
@@ -1857,16 +1857,16 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="B32" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C32" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D32" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E32" t="s">
         <v>37</v>
@@ -1874,13 +1874,13 @@
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C33" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="E33" t="s">
         <v>37</v>
@@ -1888,10 +1888,10 @@
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C34" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D34" t="s">
         <v>14</v>
@@ -1902,13 +1902,13 @@
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C35" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="D35" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E35" t="s">
         <v>15</v>
@@ -1916,41 +1916,41 @@
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C36" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="E36" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C37" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="D37" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="E37" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C38" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="D38" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E38" t="s">
         <v>8</v>
@@ -1958,13 +1958,13 @@
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C39" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="D39" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E39" t="s">
         <v>8</v>
@@ -1972,18 +1972,18 @@
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C40" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C41" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.2">
@@ -1991,10 +1991,10 @@
         <v>43</v>
       </c>
       <c r="C42" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="E42" t="s">
         <v>37</v>
@@ -2002,13 +2002,13 @@
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C43" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D43" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="E43" t="s">
         <v>37</v>
@@ -2016,10 +2016,10 @@
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C44" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="D44" t="s">
         <v>7</v>
@@ -2030,10 +2030,10 @@
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C45" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D45" t="s">
         <v>7</v>
@@ -2044,13 +2044,13 @@
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C46" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="D46" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E46" t="s">
         <v>37</v>
@@ -2058,13 +2058,13 @@
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C47" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="E47" t="s">
         <v>37</v>
@@ -2072,10 +2072,10 @@
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C48" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="D48" t="s">
         <v>14</v>
@@ -2086,13 +2086,13 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C49" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D49" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E49" t="s">
         <v>15</v>
@@ -2100,13 +2100,13 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="E50" t="s">
         <v>37</v>
@@ -2114,27 +2114,27 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C51" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="D51" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="E51" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C52" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="D52" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E52" t="s">
         <v>8</v>
@@ -2142,13 +2142,13 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C53" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="D53" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="E53" t="s">
         <v>37</v>
@@ -2156,44 +2156,44 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="C54" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="D54" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E54" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="E55" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B56" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C56" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="D56" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="E56" t="s">
         <v>8</v>
@@ -2201,10 +2201,10 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
+        <v>132</v>
+      </c>
+      <c r="C57" t="s">
         <v>137</v>
-      </c>
-      <c r="C57" t="s">
-        <v>142</v>
       </c>
       <c r="D57" t="s">
         <v>45</v>
@@ -2215,21 +2215,21 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B58" t="s">
+        <v>133</v>
+      </c>
+      <c r="C58" t="s">
         <v>138</v>
-      </c>
-      <c r="C58" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
+        <v>134</v>
+      </c>
+      <c r="C59" t="s">
         <v>139</v>
       </c>
-      <c r="C59" t="s">
-        <v>144</v>
-      </c>
       <c r="D59" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E59" t="s">
         <v>37</v>

</xml_diff>

<commit_message>
small fixes in data dic
</commit_message>
<xml_diff>
--- a/R/data_dic/data_description.xlsx
+++ b/R/data_dic/data_description.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/audhalbritter/Dropbox/Bergen/FUNDER/funcab_data/R/data_dic/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5587F406-14EF-4E4F-BE0E-7923324C209F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C26DDC1E-F5BA-CC4E-B500-377DA5B66741}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10740" yWindow="8440" windowWidth="17520" windowHeight="9380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4760" yWindow="4080" windowWidth="20040" windowHeight="12680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_description" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="142">
   <si>
     <t>TableID</t>
   </si>
@@ -492,15 +492,9 @@
     <t>Units</t>
   </si>
   <si>
-    <t>F, G, B, L</t>
-  </si>
-  <si>
     <t>Measurement was taken before or after the cut</t>
   </si>
   <si>
-    <t xml:space="preserve">Removed functional group with sampling: F = forbs, G = graminoids, B = bryophytes; L = litter </t>
-  </si>
-  <si>
     <t>Plant functional groups removed, where F = forbs, G = graminoids, B = bryophytes and C = control, and XC = extra control</t>
   </si>
   <si>
@@ -513,9 +507,6 @@
     <t>vegetation_height</t>
   </si>
   <si>
-    <t>Plant functional groups removed, where F = forbs, G = graminoids, and B = bryophytes and C = bontrol</t>
-  </si>
-  <si>
     <t>Comment on measurement</t>
   </si>
   <si>
@@ -532,6 +523,18 @@
   </si>
   <si>
     <t>PAR value of light measurement</t>
+  </si>
+  <si>
+    <t>functional_group</t>
+  </si>
+  <si>
+    <t>Removed functional group, including forbs, bryophytes, graminoids, litterm pteridophytes, lichens, and cryptograms</t>
+  </si>
+  <si>
+    <t>Removed functional group, where F = forbs, B = bryophytes, G = graminoids, L = litterm P = pteridophytes, LI = lichens, and C = cryptograms</t>
+  </si>
+  <si>
+    <t>Plant functional groups removed, where F = forbs, G = graminoids, and B = bryophytes and C = control</t>
   </si>
 </sst>
 </file>
@@ -1404,10 +1407,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E60"/>
+  <dimension ref="A1:E61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="A62" sqref="A62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1540,7 +1543,7 @@
         <v>25</v>
       </c>
       <c r="C10" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E10" t="s">
         <v>7</v>
@@ -1589,10 +1592,10 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C15" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D15" t="s">
         <v>13</v>
@@ -1606,7 +1609,7 @@
         <v>35</v>
       </c>
       <c r="C16" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>107</v>
@@ -1659,7 +1662,7 @@
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C20" t="s">
         <v>40</v>
@@ -1754,10 +1757,7 @@
         <v>54</v>
       </c>
       <c r="C27" t="s">
-        <v>129</v>
-      </c>
-      <c r="D27" t="s">
-        <v>127</v>
+        <v>140</v>
       </c>
       <c r="E27" t="s">
         <v>7</v>
@@ -1765,57 +1765,54 @@
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
-        <v>55</v>
+        <v>138</v>
       </c>
       <c r="C28" t="s">
-        <v>56</v>
-      </c>
-      <c r="D28" t="s">
-        <v>57</v>
+        <v>139</v>
       </c>
       <c r="E28" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C29" t="s">
-        <v>59</v>
+        <v>56</v>
+      </c>
+      <c r="D29" t="s">
+        <v>57</v>
       </c>
       <c r="E29" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C30" t="s">
-        <v>61</v>
+        <v>59</v>
+      </c>
+      <c r="E30" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C31" t="s">
-        <v>87</v>
-      </c>
-      <c r="D31" t="s">
-        <v>6</v>
-      </c>
-      <c r="E31" t="s">
-        <v>30</v>
+        <v>61</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C32" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D32" t="s">
         <v>6</v>
@@ -1825,31 +1822,31 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+      <c r="B33" t="s">
+        <v>63</v>
+      </c>
+      <c r="C33" t="s">
+        <v>88</v>
+      </c>
+      <c r="D33" t="s">
+        <v>6</v>
+      </c>
+      <c r="E33" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
         <v>119</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B34" t="s">
         <v>64</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C34" t="s">
         <v>98</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D34" t="s">
         <v>89</v>
-      </c>
-      <c r="E33" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B34" t="s">
-        <v>65</v>
-      </c>
-      <c r="C34" t="s">
-        <v>140</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>106</v>
       </c>
       <c r="E34" t="s">
         <v>30</v>
@@ -1857,13 +1854,13 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C35" t="s">
-        <v>138</v>
-      </c>
-      <c r="D35" t="s">
-        <v>13</v>
+        <v>137</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>106</v>
       </c>
       <c r="E35" t="s">
         <v>30</v>
@@ -1871,38 +1868,41 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C36" t="s">
-        <v>110</v>
+        <v>135</v>
       </c>
       <c r="D36" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="E36" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C37" t="s">
-        <v>91</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>101</v>
+        <v>110</v>
+      </c>
+      <c r="D37" t="s">
+        <v>41</v>
       </c>
       <c r="E37" t="s">
-        <v>100</v>
+        <v>14</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C38" t="s">
-        <v>99</v>
+        <v>91</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>101</v>
       </c>
       <c r="E38" t="s">
         <v>100</v>
@@ -1910,21 +1910,21 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C39" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="E39" t="s">
-        <v>7</v>
+        <v>100</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C40" t="s">
-        <v>109</v>
+        <v>92</v>
       </c>
       <c r="E40" t="s">
         <v>7</v>
@@ -1932,43 +1932,40 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C41" t="s">
-        <v>111</v>
+        <v>109</v>
+      </c>
+      <c r="E41" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C42" t="s">
-        <v>135</v>
+        <v>111</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C43" t="s">
-        <v>93</v>
-      </c>
-      <c r="D43" t="s">
-        <v>94</v>
-      </c>
-      <c r="E43" t="s">
-        <v>30</v>
+        <v>132</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C44" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D44" t="s">
-        <v>6</v>
+        <v>94</v>
       </c>
       <c r="E44" t="s">
         <v>30</v>
@@ -1976,10 +1973,10 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C45" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D45" t="s">
         <v>6</v>
@@ -1990,13 +1987,13 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C46" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D46" t="s">
-        <v>89</v>
+        <v>6</v>
       </c>
       <c r="E46" t="s">
         <v>30</v>
@@ -2004,13 +2001,13 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C47" t="s">
-        <v>136</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>106</v>
+        <v>97</v>
+      </c>
+      <c r="D47" t="s">
+        <v>89</v>
       </c>
       <c r="E47" t="s">
         <v>30</v>
@@ -2018,13 +2015,13 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C48" t="s">
-        <v>137</v>
-      </c>
-      <c r="D48" t="s">
-        <v>13</v>
+        <v>133</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>106</v>
       </c>
       <c r="E48" t="s">
         <v>30</v>
@@ -2032,160 +2029,174 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C49" t="s">
-        <v>90</v>
+        <v>134</v>
       </c>
       <c r="D49" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="E49" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
-        <v>81</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>101</v>
+        <v>80</v>
+      </c>
+      <c r="C50" t="s">
+        <v>90</v>
+      </c>
+      <c r="D50" t="s">
+        <v>41</v>
       </c>
       <c r="E50" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
-        <v>82</v>
-      </c>
-      <c r="C51" t="s">
-        <v>99</v>
-      </c>
-      <c r="D51" t="s">
-        <v>108</v>
+        <v>81</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>101</v>
       </c>
       <c r="E51" t="s">
-        <v>100</v>
+        <v>30</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C52" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="D52" t="s">
-        <v>53</v>
+        <v>108</v>
       </c>
       <c r="E52" t="s">
-        <v>7</v>
+        <v>100</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C53" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="D53" t="s">
-        <v>94</v>
+        <v>53</v>
       </c>
       <c r="E53" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C54" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D54" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="E54" t="s">
-        <v>100</v>
+        <v>30</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
-        <v>86</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>101</v>
+        <v>85</v>
+      </c>
+      <c r="C55" t="s">
+        <v>105</v>
+      </c>
+      <c r="D55" t="s">
+        <v>89</v>
       </c>
       <c r="E55" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
+      <c r="B56" t="s">
+        <v>86</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E56" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
         <v>120</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B57" t="s">
         <v>64</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C57" t="s">
         <v>115</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D57" t="s">
         <v>116</v>
       </c>
-      <c r="E56" t="s">
+      <c r="E57" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B57" t="s">
-        <v>112</v>
-      </c>
-      <c r="C57" t="s">
-        <v>117</v>
-      </c>
-      <c r="D57" t="s">
-        <v>36</v>
-      </c>
-      <c r="E57" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B58" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C58" t="s">
-        <v>118</v>
+        <v>117</v>
+      </c>
+      <c r="D58" t="s">
+        <v>36</v>
+      </c>
+      <c r="E58" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
+        <v>113</v>
+      </c>
+      <c r="C59" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B60" t="s">
         <v>114</v>
       </c>
-      <c r="C59" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
+      <c r="C60" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
         <v>120</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B61" t="s">
         <v>25</v>
       </c>
-      <c r="C60" t="s">
-        <v>134</v>
-      </c>
-      <c r="E60" t="s">
+      <c r="C61" t="s">
+        <v>141</v>
+      </c>
+      <c r="E61" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
make data dic for seedlings and sp biomass
</commit_message>
<xml_diff>
--- a/R/data_dic/data_description.xlsx
+++ b/R/data_dic/data_description.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/audhalbritter/Dropbox/Bergen/FUNDER/funcab_data/R/data_dic/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C26DDC1E-F5BA-CC4E-B500-377DA5B66741}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AECBB3E6-2C20-4F49-B95D-1FE44E211420}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4760" yWindow="4080" windowWidth="20040" windowHeight="12680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40420" yWindow="460" windowWidth="23840" windowHeight="19480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_description" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="153">
   <si>
     <t>TableID</t>
   </si>
@@ -535,6 +535,39 @@
   </si>
   <si>
     <t>Plant functional groups removed, where F = forbs, G = graminoids, and B = bryophytes and C = control</t>
+  </si>
+  <si>
+    <t>seedID</t>
+  </si>
+  <si>
+    <t>recruitment</t>
+  </si>
+  <si>
+    <t>Round of sampling; round 1-2 correspond to 2018, and round 3-4 to 2019</t>
+  </si>
+  <si>
+    <t>presence</t>
+  </si>
+  <si>
+    <t>Presence (1) or absence (0) of seedlings</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>x coordinate in the plot</t>
+  </si>
+  <si>
+    <t>y coordinate in the plot</t>
+  </si>
+  <si>
+    <t>sorted_by</t>
+  </si>
+  <si>
+    <t>Person that sorted the biomass</t>
   </si>
 </sst>
 </file>
@@ -1407,10 +1440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E61"/>
+  <dimension ref="A1:E67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="A62" sqref="A62"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2200,6 +2233,69 @@
         <v>7</v>
       </c>
     </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B62" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>143</v>
+      </c>
+      <c r="B63" t="s">
+        <v>51</v>
+      </c>
+      <c r="C63" t="s">
+        <v>144</v>
+      </c>
+      <c r="E63" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B64" t="s">
+        <v>145</v>
+      </c>
+      <c r="C64" t="s">
+        <v>146</v>
+      </c>
+      <c r="E64" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="65" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B65" t="s">
+        <v>147</v>
+      </c>
+      <c r="C65" t="s">
+        <v>149</v>
+      </c>
+      <c r="E65" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="66" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B66" t="s">
+        <v>148</v>
+      </c>
+      <c r="C66" t="s">
+        <v>150</v>
+      </c>
+      <c r="E66" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="67" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B67" t="s">
+        <v>151</v>
+      </c>
+      <c r="C67" t="s">
+        <v>152</v>
+      </c>
+      <c r="E67" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
add unit changes to data dic
</commit_message>
<xml_diff>
--- a/R/data_dic/data_description.xlsx
+++ b/R/data_dic/data_description.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/audhalbritter/Dropbox/Bergen/FUNDER/funcab_data/R/data_dic/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2529BB06-E9DB-E44A-94E2-237A129633AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73A4C599-945C-A243-A807-83397319AA6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33880" yWindow="460" windowWidth="27380" windowHeight="20660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10500" yWindow="460" windowWidth="27380" windowHeight="20660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_description" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="153">
   <si>
     <t>TableID</t>
   </si>
@@ -320,64 +320,6 @@
   </si>
   <si>
     <t>calculated</t>
-  </si>
-  <si>
-    <r>
-      <t>µmol mol</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="6.6"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>-1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> s</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="6.6"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">-1 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF222222"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>CO</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="6.6"/>
-        <color rgb="FF222222"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2</t>
-    </r>
   </si>
   <si>
     <t>Ecosystem respiration</t>
@@ -429,9 +371,6 @@
     </r>
   </si>
   <si>
-    <t>m3 water/m3 soil</t>
-  </si>
-  <si>
     <t>0-1</t>
   </si>
   <si>
@@ -571,13 +510,50 @@
   </si>
   <si>
     <t>Presence (1) or absence (0) of a seedling per census</t>
+  </si>
+  <si>
+    <r>
+      <t>% water content or volume water per volume soil in m</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="6.6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">3 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>m</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="6.6"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-3</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -723,21 +699,6 @@
       <vertAlign val="superscript"/>
       <sz val="6.6"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF222222"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <vertAlign val="subscript"/>
-      <sz val="6.6"/>
-      <color rgb="FF222222"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1095,7 +1056,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1453,8 +1414,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="137" workbookViewId="0">
-      <selection activeCell="D67" sqref="D67"/>
+    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="137" workbookViewId="0">
+      <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1476,7 +1437,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -1565,7 +1526,7 @@
         <v>22</v>
       </c>
       <c r="D8" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E8" t="s">
         <v>7</v>
@@ -1587,7 +1548,7 @@
         <v>25</v>
       </c>
       <c r="C10" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E10" t="s">
         <v>7</v>
@@ -1636,10 +1597,10 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C15" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D15" t="s">
         <v>13</v>
@@ -1653,10 +1614,10 @@
         <v>35</v>
       </c>
       <c r="C16" t="s">
-        <v>135</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>106</v>
+        <v>133</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>152</v>
       </c>
       <c r="E16" t="s">
         <v>30</v>
@@ -1664,7 +1625,7 @@
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C17" t="s">
         <v>37</v>
@@ -1678,7 +1639,7 @@
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C18" t="s">
         <v>38</v>
@@ -1692,7 +1653,7 @@
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C19" t="s">
         <v>39</v>
@@ -1706,7 +1667,7 @@
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C20" t="s">
         <v>40</v>
@@ -1720,7 +1681,7 @@
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C21" t="s">
         <v>42</v>
@@ -1801,7 +1762,7 @@
         <v>54</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E27" t="s">
         <v>7</v>
@@ -1809,10 +1770,10 @@
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E28" t="s">
         <v>7</v>
@@ -1823,7 +1784,7 @@
         <v>55</v>
       </c>
       <c r="C29" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D29" t="s">
         <v>56</v>
@@ -1881,7 +1842,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B34" t="s">
         <v>63</v>
@@ -1901,10 +1862,10 @@
         <v>64</v>
       </c>
       <c r="C35" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E35" t="s">
         <v>30</v>
@@ -1915,7 +1876,7 @@
         <v>65</v>
       </c>
       <c r="C36" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D36" t="s">
         <v>13</v>
@@ -1929,7 +1890,7 @@
         <v>66</v>
       </c>
       <c r="C37" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D37" t="s">
         <v>41</v>
@@ -1946,7 +1907,7 @@
         <v>90</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="E38" t="s">
         <v>99</v>
@@ -1979,7 +1940,7 @@
         <v>70</v>
       </c>
       <c r="C41" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E41" t="s">
         <v>7</v>
@@ -1990,7 +1951,7 @@
         <v>71</v>
       </c>
       <c r="C42" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
@@ -1998,7 +1959,7 @@
         <v>72</v>
       </c>
       <c r="C43" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
@@ -2062,10 +2023,10 @@
         <v>77</v>
       </c>
       <c r="C48" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E48" t="s">
         <v>30</v>
@@ -2076,7 +2037,7 @@
         <v>78</v>
       </c>
       <c r="C49" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D49" t="s">
         <v>13</v>
@@ -2104,10 +2065,10 @@
         <v>80</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="E51" t="s">
         <v>30</v>
@@ -2121,7 +2082,7 @@
         <v>98</v>
       </c>
       <c r="D52" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E52" t="s">
         <v>99</v>
@@ -2146,7 +2107,7 @@
         <v>83</v>
       </c>
       <c r="C54" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D54" t="s">
         <v>93</v>
@@ -2160,7 +2121,7 @@
         <v>84</v>
       </c>
       <c r="C55" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D55" t="s">
         <v>88</v>
@@ -2174,10 +2135,10 @@
         <v>85</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="E56" t="s">
         <v>99</v>
@@ -2185,16 +2146,16 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B57" t="s">
         <v>63</v>
       </c>
       <c r="C57" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D57" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E57" t="s">
         <v>7</v>
@@ -2202,10 +2163,10 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B58" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C58" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D58" t="s">
         <v>36</v>
@@ -2216,29 +2177,29 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C59" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B60" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C60" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B61" t="s">
         <v>25</v>
       </c>
       <c r="C61" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E61" t="s">
         <v>7</v>
@@ -2246,21 +2207,21 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B62" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C62" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B63" t="s">
         <v>51</v>
       </c>
       <c r="C63" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E63" t="s">
         <v>7</v>
@@ -2268,10 +2229,10 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B64" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E64" t="s">
         <v>30</v>
@@ -2279,10 +2240,10 @@
     </row>
     <row r="65" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B65" t="s">
+        <v>141</v>
+      </c>
+      <c r="C65" t="s">
         <v>143</v>
-      </c>
-      <c r="C65" t="s">
-        <v>145</v>
       </c>
       <c r="D65" t="s">
         <v>41</v>
@@ -2293,10 +2254,10 @@
     </row>
     <row r="66" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B66" t="s">
+        <v>142</v>
+      </c>
+      <c r="C66" t="s">
         <v>144</v>
-      </c>
-      <c r="C66" t="s">
-        <v>146</v>
       </c>
       <c r="D66" t="s">
         <v>41</v>
@@ -2307,10 +2268,10 @@
     </row>
     <row r="67" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B67" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C67" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E67" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
update time zone to UTC + 2
</commit_message>
<xml_diff>
--- a/R/data_dic/data_description.xlsx
+++ b/R/data_dic/data_description.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/audhalbritter/Dropbox/Bergen/FUNDER/funcab_data/R/data_dic/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D687F37F-641F-E64F-8154-617C616D6DDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A419B23-A777-0B48-BBB6-DFB732A078DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9520" yWindow="460" windowWidth="18820" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -544,22 +544,22 @@
     </r>
   </si>
   <si>
-    <t>Date and time of sampling (UTC)</t>
-  </si>
-  <si>
-    <t>Time of sampling  (UTC)</t>
-  </si>
-  <si>
-    <t>Time in seconds for dark measurement  (UTC)</t>
-  </si>
-  <si>
-    <t>PAR value of dark measurement  (UTC)</t>
-  </si>
-  <si>
-    <t>Start time of light measurement  (UTC)</t>
-  </si>
-  <si>
-    <t>End time of light measurement (UTC)</t>
+    <t>Time of sampling  (UTC + 2)</t>
+  </si>
+  <si>
+    <t>PAR value of dark measurement  (UTC + 2)</t>
+  </si>
+  <si>
+    <t>Time in seconds for dark measurement  (UTC + 2)</t>
+  </si>
+  <si>
+    <t>End time of light measurement (UTC + 2)</t>
+  </si>
+  <si>
+    <t>Start time of light measurement  (UTC + 2)</t>
+  </si>
+  <si>
+    <t>Date and time of sampling (UTC + 2)</t>
   </si>
 </sst>
 </file>
@@ -1444,7 +1444,7 @@
   <dimension ref="A1:E67"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="137" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1477,7 +1477,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="D2" t="s">
         <v>5</v>
@@ -1863,7 +1863,7 @@
         <v>61</v>
       </c>
       <c r="C33" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D33" t="s">
         <v>5</v>
@@ -2055,7 +2055,7 @@
         <v>76</v>
       </c>
       <c r="C48" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>100</v>
@@ -2184,7 +2184,7 @@
         <v>62</v>
       </c>
       <c r="C57" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D57" t="s">
         <v>108</v>

</xml_diff>